<commit_message>
commit tsy 29.03 b/c wanna pull like
</commit_message>
<xml_diff>
--- a/Unit_Data.xlsx
+++ b/Unit_Data.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Name</t>
   </si>
@@ -70,6 +70,9 @@
   </si>
   <si>
     <t>Caiman</t>
+  </si>
+  <si>
+    <t>WA</t>
   </si>
 </sst>
 </file>
@@ -411,7 +414,7 @@
   <dimension ref="A1:P4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T15" sqref="S15:T15"/>
+      <selection activeCell="S12" sqref="S12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -455,7 +458,7 @@
         <v>11</v>
       </c>
       <c r="L1" t="s">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="M1" t="s">
         <v>12</v>

</xml_diff>